<commit_message>
meet and classroom will open in separate tabs
</commit_message>
<xml_diff>
--- a/timetable.xlsx
+++ b/timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anves\Documents\G-Class-Automator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59E0419-791F-4644-8CC6-B9E883CD0C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE703AE-4685-48EE-AD9E-748D79CAD5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="u2hjap5n6n+XL7uvnfu9J3mH1JsSoxEQQ+dlLQHGzZb/+/UFcL9ZNcwxUeml6hhMyS+xQixhy8mp8DSBQJL7Hw==" workbookSaltValue="am7EwL4UQSME5bpAoYJdQw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3324F5EB-7482-46E8-BC0B-7B6FDC17CDB5}"/>
@@ -49,7 +49,7 @@
     <t>Subject Abbreviation</t>
   </si>
   <si>
-    <t>Lecture start time (HH:MM:SS)</t>
+    <t>Lecture start time</t>
   </si>
 </sst>
 </file>
@@ -92,7 +92,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -205,7 +205,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FF5F803-BAA1-4F65-9C0C-39249EEF306E}" name="Table2" displayName="Table2" ref="A1:F8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:F8" xr:uid="{8FF5F803-BAA1-4F65-9C0C-39249EEF306E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{339E21A3-1F16-41C4-B8A3-21BF3523D03B}" name="Lecture start time (HH:MM:SS)" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{339E21A3-1F16-41C4-B8A3-21BF3523D03B}" name="Lecture start time" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{FCDDDC18-D6A1-4769-BBCB-BA9D1022E144}" name="Monday" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{BBAA38B2-B887-444E-BD02-732F0C8B6E84}" name="Tuesday" dataDxfId="7"/>
     <tableColumn id="4" xr3:uid="{59AC9EE2-D344-4B22-8FA6-4ED6535C039A}" name="Wednesday" dataDxfId="6"/>
@@ -592,7 +592,7 @@
     <row r="9" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fB3yw5jfr34428DcWDiu9pWabOckS3kMMqW+1fdOm3xGas/iEUeOmQAWw3wveZWzaWvhexXisNLBAUbMm2s7YA==" saltValue="302WS0fzh93Zm3zziw4QCA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/a8Yzf+L8/6M83JpI1AbG6L66hhBBUHuhjlErCcANrQ7vSbKraOd+pSlqiOoG9kirpDKJJaY9eh6qvHnoTr+bg==" saltValue="I17k8I/qDc43vbTOIXWGIw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>